<commit_message>
Added IOPC services concordance
</commit_message>
<xml_diff>
--- a/beef_production_IOPC2009_conc_make.xlsx
+++ b/beef_production_IOPC2009_conc_make.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27713"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10909"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobfry/Desktop/Project/LIEF/concordances/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobfry/Desktop/Projects/uni_projects/LIEF/concordances/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0836FE6-4F17-7948-B252-5375D06E078A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="-6920" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -3893,7 +3894,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -3929,6 +3930,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3990,17 +3992,7 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -4026,6 +4018,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -4352,14 +4347,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AWL4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="AK3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="AVT3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AM4" sqref="AM4"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3:AWK4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13967,7 +13962,7 @@
         <v>0</v>
       </c>
       <c r="XF3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="XG3">
         <v>0</v>
@@ -15936,7 +15931,7 @@
       </c>
       <c r="AWL3">
         <f>SUM(B3:AWK3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1286" x14ac:dyDescent="0.2">
@@ -19802,12 +19797,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:AWK4">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AWL3:AWL4">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>